<commit_message>
Vytvorenie administracie - moznost vytvorit a dropnut databazu
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6047FDA4-FDED-402B-A1CF-A43D1BE657AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1E1E47-1609-4529-886C-F25E608B5839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{945F86FC-0632-4044-B9F2-D6FB8DDFB35B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{945F86FC-0632-4044-B9F2-D6FB8DDFB35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>uid</t>
   </si>
@@ -48,9 +48,6 @@
     <t>lname</t>
   </si>
   <si>
-    <t>company</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>page</t>
   </si>
   <si>
-    <t>"h"/"t"</t>
-  </si>
-  <si>
     <t>HOME / TECHNOLOGY</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>message</t>
   </si>
   <si>
-    <t>MESSAGES_ATTACH</t>
-  </si>
-  <si>
     <t>aid</t>
   </si>
   <si>
@@ -184,6 +175,33 @@
   </si>
   <si>
     <t>add_info</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>comp</t>
+  </si>
+  <si>
+    <t>change_date</t>
+  </si>
+  <si>
+    <t>true/false</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>create_date_m</t>
+  </si>
+  <si>
+    <t>MESSAGE_ATTACH</t>
   </si>
 </sst>
 </file>
@@ -557,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAFC533-038C-464D-B642-824FE1C70B4C}">
-  <dimension ref="B5:T28"/>
+  <dimension ref="B5:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,23 +595,24 @@
     <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
@@ -604,25 +623,25 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L6" t="s">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="T6" t="s">
         <v>1</v>
@@ -636,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
         <v>2</v>
@@ -645,19 +664,19 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="T7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.25">
@@ -665,146 +684,168 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="L8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" t="s">
-        <v>17</v>
-      </c>
       <c r="O8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="S9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="D13" t="s">
-        <v>19</v>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H23" t="s">
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L23" t="s">
         <v>1</v>
       </c>
       <c r="O23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P23" t="s">
         <v>1</v>
       </c>
       <c r="S23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="T23" t="s">
         <v>1</v>
@@ -812,93 +853,118 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
         <v>37</v>
       </c>
-      <c r="D24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" t="s">
-        <v>39</v>
-      </c>
       <c r="G24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K24" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="O24" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="P24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="T24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
         <v>32</v>
       </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" t="s">
-        <v>33</v>
-      </c>
       <c r="K25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O25" t="s">
         <v>0</v>
       </c>
-      <c r="L25" t="s">
-        <v>24</v>
-      </c>
-      <c r="O25" t="s">
-        <v>46</v>
-      </c>
       <c r="P25" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H26" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" t="s">
         <v>19</v>
       </c>
-      <c r="K26" t="s">
-        <v>20</v>
-      </c>
       <c r="L26" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="O26" t="s">
+        <v>44</v>
+      </c>
+      <c r="P26" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="O27" t="s">
+        <v>57</v>
+      </c>
+      <c r="P27" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vytvorenie menu a stranok
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1E1E47-1609-4529-886C-F25E608B5839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D609FBFC-8667-4C2D-B308-D74DD8C6965D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{945F86FC-0632-4044-B9F2-D6FB8DDFB35B}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>HOME / TECHNOLOGY</t>
   </si>
   <si>
-    <t>GALERY</t>
-  </si>
-  <si>
     <t>iid</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>MESSAGE_ATTACH</t>
+  </si>
+  <si>
+    <t>GALLERY</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="B5:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
         <v>25</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
         <v>28</v>
       </c>
       <c r="S6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T6" t="s">
         <v>1</v>
@@ -673,7 +673,7 @@
         <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T7" t="s">
         <v>8</v>
@@ -708,7 +708,7 @@
         <v>8</v>
       </c>
       <c r="S8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T8" t="s">
         <v>8</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -734,7 +734,7 @@
         <v>18</v>
       </c>
       <c r="S9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T9" t="s">
         <v>18</v>
@@ -762,15 +762,15 @@
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -807,16 +807,16 @@
         <v>35</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O22" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="S22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" t="s">
         <v>1</v>
@@ -839,13 +839,13 @@
         <v>1</v>
       </c>
       <c r="O23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P23" t="s">
         <v>1</v>
       </c>
       <c r="S23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T23" t="s">
         <v>1</v>
@@ -856,7 +856,7 @@
         <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
         <v>37</v>
@@ -877,7 +877,7 @@
         <v>23</v>
       </c>
       <c r="S24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T24" t="s">
         <v>23</v>
@@ -926,7 +926,7 @@
         <v>18</v>
       </c>
       <c r="O26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P26" t="s">
         <v>8</v>
@@ -940,7 +940,7 @@
         <v>8</v>
       </c>
       <c r="O27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P27" t="s">
         <v>18</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">

</xml_diff>